<commit_message>
department duplicate company based
</commit_message>
<xml_diff>
--- a/src/assets/files/AssetUpload.xlsx
+++ b/src/assets/files/AssetUpload.xlsx
@@ -196,7 +196,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,14 +217,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -312,51 +318,29 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -390,6 +374,30 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -404,25 +412,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L6" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:L6">
     <filterColumn colId="9"/>
     <filterColumn colId="10"/>
     <filterColumn colId="11"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="Asset Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Asset Code" dataDxfId="10"/>
-    <tableColumn id="3" name="Asset Location" dataDxfId="9"/>
-    <tableColumn id="4" name="Asset Category" dataDxfId="8"/>
-    <tableColumn id="16" name="Capitalization Price" dataDxfId="7"/>
-    <tableColumn id="17" name="Capitalization Date" dataDxfId="6"/>
-    <tableColumn id="18" name="Life in years" dataDxfId="5"/>
-    <tableColumn id="19" name="Salvage Value" dataDxfId="4"/>
-    <tableColumn id="20" name="Depreciation%" dataDxfId="3"/>
+    <tableColumn id="1" name="Asset Name" dataDxfId="10"/>
+    <tableColumn id="2" name="Asset Code" dataDxfId="9"/>
+    <tableColumn id="3" name="Asset Location" dataDxfId="8"/>
+    <tableColumn id="4" name="Asset Category" dataDxfId="7"/>
+    <tableColumn id="16" name="Capitalization Price" dataDxfId="6"/>
+    <tableColumn id="17" name="Capitalization Date" dataDxfId="5"/>
+    <tableColumn id="18" name="Life in years" dataDxfId="4"/>
+    <tableColumn id="19" name="Salvage Value" dataDxfId="3"/>
+    <tableColumn id="20" name="Depreciation%" dataDxfId="2"/>
     <tableColumn id="5" name="Status"/>
-    <tableColumn id="26" name="Put Use Date" dataDxfId="2"/>
-    <tableColumn id="27" name="Asset User" dataDxfId="1"/>
+    <tableColumn id="26" name="Put Use Date" dataDxfId="1"/>
+    <tableColumn id="27" name="Asset User" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -716,7 +724,7 @@
   <dimension ref="A1:AR999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="A2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -749,208 +757,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="8"/>
+      <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:44">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:44">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:44">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:44">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:44">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="M6" s="4"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:44">
       <c r="A7" s="1"/>
@@ -1015,19 +1025,19 @@
       </c>
     </row>
     <row r="11" spans="1:44">
-      <c r="AO11" s="5"/>
-      <c r="AQ11" s="5"/>
-      <c r="AR11" s="4"/>
+      <c r="AO11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="3"/>
     </row>
     <row r="13" spans="1:44">
-      <c r="AO13" s="5"/>
-      <c r="AQ13" s="5"/>
-      <c r="AR13" s="4"/>
+      <c r="AO13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="3"/>
     </row>
     <row r="14" spans="1:44">
-      <c r="AO14" s="5"/>
-      <c r="AQ14" s="5"/>
-      <c r="AR14" s="4"/>
+      <c r="AO14" s="4"/>
+      <c r="AQ14" s="4"/>
+      <c r="AR14" s="3"/>
     </row>
     <row r="15" spans="1:44">
       <c r="A15" s="1"/>

</xml_diff>